<commit_message>
Implicit wait ,Assertion,Cross browser using if ,else
</commit_message>
<xml_diff>
--- a/src/test/java/TestData/Nopcomdtadriven.xlsx
+++ b/src/test/java/TestData/Nopcomdtadriven.xlsx
@@ -5,14 +5,15 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PragatiSharma\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PragatiSharma\IdeaProjects\NopCommerceBddPropertiesAndExcel\src\test\java\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4035"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4035" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
   <si>
     <t>Fname</t>
   </si>
@@ -57,6 +58,30 @@
   </si>
   <si>
     <t>qwerty123</t>
+  </si>
+  <si>
+    <t>Amit</t>
+  </si>
+  <si>
+    <t>Sharma</t>
+  </si>
+  <si>
+    <t>Add</t>
+  </si>
+  <si>
+    <t>Xyxsaa</t>
+  </si>
+  <si>
+    <t>ConfPass</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>wrty45678</t>
+  </si>
+  <si>
+    <t>praga11@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -387,7 +412,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
@@ -445,4 +470,66 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="28" customWidth="1"/>
+    <col min="4" max="4" width="21.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>